<commit_message>
Finishing up the new update
</commit_message>
<xml_diff>
--- a/resources/data-imports/Core Imports/class-specials.xlsx
+++ b/resources/data-imports/Core Imports/class-specials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="312">
   <si>
     <t>id</t>
   </si>
@@ -897,6 +897,60 @@
   </si>
   <si>
     <t>Deal 75,000 damage growing by 750 for an additional 75,000 damage as well as adding 30% of your damage stat as bonus damage. Procs while using ANY attack. Grow all your attributes, see below, by +200% over time.</t>
+  </si>
+  <si>
+    <t>Pale Whisper</t>
+  </si>
+  <si>
+    <t>Increase your Damage and Healing by +50% at level 100.</t>
+  </si>
+  <si>
+    <t>Tincture of Faith</t>
+  </si>
+  <si>
+    <t>Grow your healing by +200% at level 100.</t>
+  </si>
+  <si>
+    <t>Hollow Existance</t>
+  </si>
+  <si>
+    <t>Grow your damage by +75%, your AC (defence) by +100% and your healing by +250% at level 100.</t>
+  </si>
+  <si>
+    <t>Chalice of suffering</t>
+  </si>
+  <si>
+    <t>Increase damage by +100%, Healing by +250% and Health by +200% at level 100</t>
+  </si>
+  <si>
+    <t>Cornered in a fight</t>
+  </si>
+  <si>
+    <t>Increase your damage by +300% at level 100</t>
+  </si>
+  <si>
+    <t>Faithless Aboration</t>
+  </si>
+  <si>
+    <t>Increase your healing by +300% at level 100 and your spell damage by +150% at level 100.</t>
+  </si>
+  <si>
+    <t>Graverobbing Shadows of Pain</t>
+  </si>
+  <si>
+    <t>Deal damage equal to 2500 + 2.5% of your damage, growing by a total of +2500 at level 100</t>
+  </si>
+  <si>
+    <t>Necroctic Emotional Drift</t>
+  </si>
+  <si>
+    <t>Deal 8,000 damage + 6% of your damage stat as damage with a bonus of +8,000 damage at level 100. You will also grow your damage modifier by +200% at level 100.</t>
+  </si>
+  <si>
+    <t>The line between life and death</t>
+  </si>
+  <si>
+    <t>Deal 20,000 damage while use 20% of yuor damage stat, growing to +20,000 damage at level 100. You will also grow your damage stat by +200% at level 100.</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1290,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:T135"/>
+  <dimension ref="A1:T144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -5544,6 +5598,240 @@
         <v>22</v>
       </c>
     </row>
+    <row r="136" spans="1:20">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>16</v>
+      </c>
+      <c r="C136" t="s">
+        <v>294</v>
+      </c>
+      <c r="D136" t="s">
+        <v>295</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+      <c r="I136">
+        <v>0.05</v>
+      </c>
+      <c r="K136">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>16</v>
+      </c>
+      <c r="C137" t="s">
+        <v>296</v>
+      </c>
+      <c r="D137" t="s">
+        <v>297</v>
+      </c>
+      <c r="E137">
+        <v>12</v>
+      </c>
+      <c r="K137">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>16</v>
+      </c>
+      <c r="C138" t="s">
+        <v>298</v>
+      </c>
+      <c r="D138" t="s">
+        <v>299</v>
+      </c>
+      <c r="E138">
+        <v>24</v>
+      </c>
+      <c r="I138">
+        <v>0.0075</v>
+      </c>
+      <c r="J138">
+        <v>0.01</v>
+      </c>
+      <c r="K138">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>16</v>
+      </c>
+      <c r="C139" t="s">
+        <v>300</v>
+      </c>
+      <c r="D139" t="s">
+        <v>301</v>
+      </c>
+      <c r="E139">
+        <v>36</v>
+      </c>
+      <c r="K139">
+        <v>0.025</v>
+      </c>
+      <c r="M139">
+        <v>0.02</v>
+      </c>
+      <c r="N139">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>16</v>
+      </c>
+      <c r="C140" t="s">
+        <v>302</v>
+      </c>
+      <c r="D140" t="s">
+        <v>303</v>
+      </c>
+      <c r="E140">
+        <v>48</v>
+      </c>
+      <c r="N140">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>16</v>
+      </c>
+      <c r="C141" t="s">
+        <v>304</v>
+      </c>
+      <c r="D141" t="s">
+        <v>305</v>
+      </c>
+      <c r="E141">
+        <v>60</v>
+      </c>
+      <c r="K141">
+        <v>0.03</v>
+      </c>
+      <c r="L141">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>16</v>
+      </c>
+      <c r="C142" t="s">
+        <v>306</v>
+      </c>
+      <c r="D142" t="s">
+        <v>307</v>
+      </c>
+      <c r="E142">
+        <v>70</v>
+      </c>
+      <c r="F142">
+        <v>2500</v>
+      </c>
+      <c r="G142">
+        <v>25</v>
+      </c>
+      <c r="H142">
+        <v>0.025</v>
+      </c>
+      <c r="O142" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>16</v>
+      </c>
+      <c r="C143" t="s">
+        <v>308</v>
+      </c>
+      <c r="D143" t="s">
+        <v>309</v>
+      </c>
+      <c r="E143">
+        <v>80</v>
+      </c>
+      <c r="F143">
+        <v>8000</v>
+      </c>
+      <c r="G143">
+        <v>80</v>
+      </c>
+      <c r="H143">
+        <v>0.06</v>
+      </c>
+      <c r="I143">
+        <v>0.02</v>
+      </c>
+      <c r="O143" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>16</v>
+      </c>
+      <c r="C144" t="s">
+        <v>310</v>
+      </c>
+      <c r="D144" t="s">
+        <v>311</v>
+      </c>
+      <c r="E144">
+        <v>90</v>
+      </c>
+      <c r="F144">
+        <v>20000</v>
+      </c>
+      <c r="G144">
+        <v>200</v>
+      </c>
+      <c r="H144">
+        <v>0.12</v>
+      </c>
+      <c r="I144">
+        <v>0.02</v>
+      </c>
+      <c r="N144">
+        <v>0.02</v>
+      </c>
+      <c r="O144" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>